<commit_message>
update files and db
</commit_message>
<xml_diff>
--- a/screenshots/MAGNAreport.xlsx
+++ b/screenshots/MAGNAreport.xlsx
@@ -10,13 +10,16 @@
     <sheet name="Cihazlar" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Servis Kayıtları" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Arıza Kayıtları" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Özet" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Marka-Sağlam" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Marka-Arızalı" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Marka-Serviste" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Tip-Sağlam" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Tip-Arızalı" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Tip-Serviste" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Kullanımda" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Özet" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Marka-Sağlam" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Marka-Arızalı" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Marka-Serviste" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Marka-Kullanımda" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Tip-Sağlam" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Tip-Arızalı" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Tip-Serviste" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Tip-Kullanımda" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -908,7 +911,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Hayır</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1313,6 +1316,181 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tip</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Smartphone</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Adapter 20W</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tip</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Smartphone</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Monitor</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tip</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Smartphone</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1333,7 +1511,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Değer</t>
+          <t>Tip</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1345,21 +1523,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Smartphone</t>
+          <t>Laptop</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Laptop</t>
+          <t>Smartphone</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1480,7 +1658,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Beklemede</t>
+          <t>Tamir Edildi</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -1491,7 +1669,11 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
           <t>2025-08-22</t>
@@ -1948,7 +2130,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Evet</t>
+          <t>Hayır</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1956,7 +2138,11 @@
           <t>2025-08-22</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2025-08-28 11:43:15</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -2047,7 +2233,201 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="11" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Kullanım ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Kullanıcı</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Veriliş Tarihi</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cihaz ID</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Marka</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Tip</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Seri No</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Home Code</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>OS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ahmet Denizoğlu</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Toshiba</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>COMP-QP34-2025-033</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>SUA456732</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Windows 10 Pro</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Erdenay Çubukçu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-08-13</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Apple Iphone 8</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Smartphone</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>490154203165432</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nevra Kurt</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>16</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Apple Iphone 13</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Smartphone</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>351756059874123</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2074,40 +2454,50 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sağlam Depoda</t>
+          <t>Kullanımda</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Arızalı Depoda</t>
+          <t>Serviste</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Serviste</t>
+          <t>Arızalı Depoda</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Toplam</t>
+          <t>Sağlam Depoda</t>
         </is>
       </c>
       <c r="B5" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Toplam Cihaz</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>21</v>
       </c>
     </row>
@@ -2116,7 +2506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2137,7 +2527,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Değer</t>
+          <t>Marka</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -2163,7 +2553,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -2241,13 +2631,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2262,7 +2652,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Değer</t>
+          <t>Marka</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -2304,20 +2694,10 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dell Latitude</t>
+          <t>Monster</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Monster</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2326,13 +2706,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2347,7 +2727,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Değer</t>
+          <t>Marka</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -2364,81 +2744,6 @@
       </c>
       <c r="B2" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Dell Latitude</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="6" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Değer</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Adet</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Smartphone</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Laptop</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Adapter 20W</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2460,14 +2765,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Değer</t>
+          <t>Marka</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -2479,17 +2784,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Smartphone</t>
+          <t>Toshiba</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Monitor</t>
+          <t>Apple Iphone 8</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2499,11 +2804,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Laptop</t>
+          <t>Apple Iphone 13</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>